<commit_message>
Reviewed Driver and Publication User Stories
</commit_message>
<xml_diff>
--- a/User Stories/Driver&PubUserStories.xlsx
+++ b/User Stories/Driver&PubUserStories.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbcdef5057a82b24/Documents/GitHub/Newsagent-Project/User Stories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Palej\Desktop\Software Design with AI for Cloud\Year_3\agile-labs3\Newsagent-Project\User Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{0CAC537A-D0F5-44B4-B8C1-590AB52AA478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AF8595F-C60F-4F5B-A81F-5E35CCE0F957}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394DACC3-B259-496C-B6F7-60447024E19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{6F4168C7-28B8-4B96-A04E-7170FD7B4563}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{6F4168C7-28B8-4B96-A04E-7170FD7B4563}"/>
   </bookViews>
   <sheets>
     <sheet name="DeliveryDriver" sheetId="1" r:id="rId1"/>
@@ -36,8 +36,39 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={07A4A8D0-1216-402B-9430-E2C4A10A537D}</author>
+    <author>tc={8EF8B2DF-F020-4E31-8A9A-05BEDC38B1C1}</author>
+  </authors>
+  <commentList>
+    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{07A4A8D0-1216-402B-9430-E2C4A10A537D}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Make it more descriptive, verify when not delivered +1 quantity, verify when delivered -1 from quantity 
+</t>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="1" shapeId="0" xr:uid="{8EF8B2DF-F020-4E31-8A9A-05BEDC38B1C1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    I would add extra struff like:
+Verify date correct
+Verify invoice printed for each customer 
+etc</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>Acceptance Criteria</t>
   </si>
@@ -141,29 +172,50 @@
     <t>As a Newsagent</t>
   </si>
   <si>
-    <t>I want to read the details of the publication book</t>
-  </si>
-  <si>
-    <t>so I can check publications if customers have any questions</t>
-  </si>
-  <si>
-    <t>so I can give the relevant info to a customer or delivery driver</t>
-  </si>
-  <si>
-    <t>I want to read the stock level of each publication</t>
+    <t>Stock +1 when not delivered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stock -1 when delivered </t>
+  </si>
+  <si>
+    <t>Publication details include:</t>
+  </si>
+  <si>
+    <t>title name, author, price, quantity</t>
+  </si>
+  <si>
+    <t>I want to read stock details</t>
+  </si>
+  <si>
+    <t>I want to add publication to stock</t>
+  </si>
+  <si>
+    <t>I want to remove publication from warehouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I want to update publication price </t>
+  </si>
+  <si>
+    <t>so I keep accurate stock information</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -195,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -209,6 +261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -216,11 +269,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -238,6 +286,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Natalia Palej" id="{E65FAB13-016D-4910-9A30-F5E3864FEAC0}" userId="cad1acabf18afac6" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -535,38 +589,53 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D14" dT="2023-10-05T12:47:27.65" personId="{E65FAB13-016D-4910-9A30-F5E3864FEAC0}" id="{07A4A8D0-1216-402B-9430-E2C4A10A537D}">
+    <text xml:space="preserve">Make it more descriptive, verify when not delivered +1 quantity, verify when delivered -1 from quantity 
+</text>
+  </threadedComment>
+  <threadedComment ref="D16" dT="2023-10-05T12:48:35.37" personId="{E65FAB13-016D-4910-9A30-F5E3864FEAC0}" id="{8EF8B2DF-F020-4E31-8A9A-05BEDC38B1C1}">
+    <text>I would add extra struff like:
+Verify date correct
+Verify invoice printed for each customer 
+etc</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE66FCB5-4BF4-4903-BAAB-3414C50CE758}">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE66FCB5-4BF4-4903-BAAB-3414C50CE758}">
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -576,10 +645,10 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D2" s="8"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -596,7 +665,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -604,7 +673,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -612,7 +681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -621,7 +690,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -635,12 +704,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
         <v>18</v>
       </c>
@@ -648,7 +717,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
         <v>11</v>
       </c>
@@ -656,12 +725,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D12" t="s">
         <v>21</v>
       </c>
@@ -669,12 +738,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D13" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -690,13 +759,19 @@
       <c r="E14" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -718,40 +793,44 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9DD4A9-7F47-415E-AA8D-1892EEF1F04A}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.46484375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.265625" customWidth="1"/>
+    <col min="7" max="7" width="3.06640625" customWidth="1"/>
+    <col min="8" max="8" width="23.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -761,29 +840,44 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>33</v>
       </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Driver&PubUS to help me understand them
</commit_message>
<xml_diff>
--- a/User Stories/Driver&PubUserStories.xlsx
+++ b/User Stories/Driver&PubUserStories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbcdef5057a82b24/Documents/GitHub/Newsagent-Project/User Stories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{394DACC3-B259-496C-B6F7-60447024E19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E3BB432-7D19-43F0-8816-E104D3A971C0}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{394DACC3-B259-496C-B6F7-60447024E19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64E7D2CE-C965-4930-8FEA-44067DC8E256}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6F4168C7-28B8-4B96-A04E-7170FD7B4563}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{6F4168C7-28B8-4B96-A04E-7170FD7B4563}"/>
   </bookViews>
   <sheets>
     <sheet name="DeliveryDriver" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <author>tc={8EF8B2DF-F020-4E31-8A9A-05BEDC38B1C1}</author>
   </authors>
   <commentList>
-    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{07A4A8D0-1216-402B-9430-E2C4A10A537D}">
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{07A4A8D0-1216-402B-9430-E2C4A10A537D}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -52,7 +52,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="D18" authorId="1" shapeId="0" xr:uid="{8EF8B2DF-F020-4E31-8A9A-05BEDC38B1C1}">
+    <comment ref="D20" authorId="1" shapeId="0" xr:uid="{8EF8B2DF-F020-4E31-8A9A-05BEDC38B1C1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>Acceptance Criteria</t>
   </si>
@@ -187,16 +187,37 @@
     <t>I want to read stock details</t>
   </si>
   <si>
-    <t>I want to add publication to stock</t>
-  </si>
-  <si>
-    <t>I want to remove publication from warehouse</t>
-  </si>
-  <si>
     <t xml:space="preserve">I want to update publication price </t>
   </si>
   <si>
     <t>so I keep accurate stock information</t>
+  </si>
+  <si>
+    <t>Verify date correct</t>
+  </si>
+  <si>
+    <t>Verify invoice printed for correct customer</t>
+  </si>
+  <si>
+    <t>Verify publication details are correct</t>
+  </si>
+  <si>
+    <t>I want to update stock on the system</t>
+  </si>
+  <si>
+    <t>so I can make a profit</t>
+  </si>
+  <si>
+    <t>Verify stock updates by correct amount</t>
+  </si>
+  <si>
+    <t>Verify the publication price updates ny correct amount</t>
+  </si>
+  <si>
+    <t>Verify that stock &gt;= 0</t>
+  </si>
+  <si>
+    <t>Verify price is &gt;= €0.00</t>
   </si>
 </sst>
 </file>
@@ -585,11 +606,11 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D14" dT="2023-10-05T12:47:27.65" personId="{E65FAB13-016D-4910-9A30-F5E3864FEAC0}" id="{07A4A8D0-1216-402B-9430-E2C4A10A537D}">
+  <threadedComment ref="D17" dT="2023-10-05T12:47:27.65" personId="{E65FAB13-016D-4910-9A30-F5E3864FEAC0}" id="{07A4A8D0-1216-402B-9430-E2C4A10A537D}">
     <text xml:space="preserve">Make it more descriptive, verify when not delivered +1 quantity, verify when delivered -1 from quantity 
 </text>
   </threadedComment>
-  <threadedComment ref="D18" dT="2023-10-05T12:48:35.37" personId="{E65FAB13-016D-4910-9A30-F5E3864FEAC0}" id="{8EF8B2DF-F020-4E31-8A9A-05BEDC38B1C1}">
+  <threadedComment ref="D20" dT="2023-10-05T12:48:35.37" personId="{E65FAB13-016D-4910-9A30-F5E3864FEAC0}" id="{8EF8B2DF-F020-4E31-8A9A-05BEDC38B1C1}">
     <text>I would add extra struff like:
 Verify date correct
 Verify invoice printed for each customer 
@@ -600,23 +621,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE66FCB5-4BF4-4903-BAAB-3414C50CE758}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="A15:XFD15"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="66.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
@@ -629,7 +650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -642,7 +663,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -659,7 +680,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -667,7 +688,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -675,7 +696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -684,99 +705,127 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D9" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C10" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D11" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D12" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
         <v>21</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D13" s="2" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D15" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>4</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B17" t="s">
         <v>24</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" t="s">
         <v>27</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D17" t="s">
         <v>29</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E17" t="s">
         <v>30</v>
       </c>
-      <c r="F14" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D17" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>4</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>25</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>28</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D20" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D22" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -793,9 +842,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9DD4A9-7F47-415E-AA8D-1892EEF1F04A}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -804,7 +853,7 @@
     <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.26953125" customWidth="1"/>
     <col min="7" max="7" width="3.08984375" customWidth="1"/>
@@ -845,7 +894,10 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
       </c>
       <c r="E3" t="s">
         <v>36</v>
@@ -856,6 +908,30 @@
         <v>37</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>33</v>
@@ -863,15 +939,21 @@
       <c r="B12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B24" t="s">
-        <v>41</v>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ronanBranch created and Pub UML made
</commit_message>
<xml_diff>
--- a/User Stories/Driver&PubUserStories.xlsx
+++ b/User Stories/Driver&PubUserStories.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbcdef5057a82b24/Documents/GitHub/Newsagent-Project/User Stories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{394DACC3-B259-496C-B6F7-60447024E19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E703E33-AA89-4FCB-B048-4CADB54B1449}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="13_ncr:1_{394DACC3-B259-496C-B6F7-60447024E19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA6AE2C1-4B68-4B4A-A623-7D8ADDC06023}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6F4168C7-28B8-4B96-A04E-7170FD7B4563}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{6F4168C7-28B8-4B96-A04E-7170FD7B4563}"/>
   </bookViews>
   <sheets>
     <sheet name="DeliveryDriver" sheetId="1" r:id="rId1"/>
     <sheet name="PublicationBook" sheetId="2" r:id="rId2"/>
+    <sheet name="UMLs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="74">
   <si>
     <t>Acceptance Criteria</t>
   </si>
@@ -169,15 +170,9 @@
     <t>Publication details include:</t>
   </si>
   <si>
-    <t>title name, author, price, quantity</t>
-  </si>
-  <si>
     <t>I want to read stock details</t>
   </si>
   <si>
-    <t xml:space="preserve">I want to update publication price </t>
-  </si>
-  <si>
     <t>so I keep accurate stock information</t>
   </si>
   <si>
@@ -193,9 +188,6 @@
     <t>I want to update stock on the system</t>
   </si>
   <si>
-    <t>so I can make a profit</t>
-  </si>
-  <si>
     <t>Verify stock updates by correct amount</t>
   </si>
   <si>
@@ -221,13 +213,91 @@
   </si>
   <si>
     <t>Verify deliveryStatus is updated</t>
+  </si>
+  <si>
+    <t>Publication</t>
+  </si>
+  <si>
+    <t>- title : String</t>
+  </si>
+  <si>
+    <t>title name, author, price, quantity, id, issue no</t>
+  </si>
+  <si>
+    <t>- publicationDatabase: Database</t>
+  </si>
+  <si>
+    <t>- issueNo : int</t>
+  </si>
+  <si>
+    <t>- id : int</t>
+  </si>
+  <si>
+    <t>- author : String</t>
+  </si>
+  <si>
+    <t>- price : double</t>
+  </si>
+  <si>
+    <t>- quantity : int</t>
+  </si>
+  <si>
+    <t>+Publication : (id: int, title: String, issueNo: int, author: String, price: double, quantity: int, publicationDatabase: Database)</t>
+  </si>
+  <si>
+    <t>I want to create a new publication</t>
+  </si>
+  <si>
+    <t>so a customer can see a new newspaper etc</t>
+  </si>
+  <si>
+    <t>Verify that new publication object is created</t>
+  </si>
+  <si>
+    <t>Verify that most of new publication details are unique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I want to update publication details </t>
+  </si>
+  <si>
+    <t>so I don't have a problem</t>
+  </si>
+  <si>
+    <t>I want to delete a publication</t>
+  </si>
+  <si>
+    <t>so I can save time</t>
+  </si>
+  <si>
+    <t>Verify that publication is deleted from database</t>
+  </si>
+  <si>
+    <t>Verify that new publication tuple is created</t>
+  </si>
+  <si>
+    <t>Verify that publication object is deleted</t>
+  </si>
+  <si>
+    <t>+createNewPublication(id: int, title: String, issueNo: int, author: String, price: double, quantity: int)</t>
+  </si>
+  <si>
+    <t>+readPublication() : void</t>
+  </si>
+  <si>
+    <t>+deletePublication() : void</t>
+  </si>
+  <si>
+    <t>+updateStock() : void</t>
+  </si>
+  <si>
+    <t>+updateCustomer (id: int, title: String, issueNo: int, author: String, price: double, quantity: int)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,16 +305,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -261,11 +344,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -289,6 +409,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE66FCB5-4BF4-4903-BAAB-3414C50CE758}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -785,23 +918,23 @@
         <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
         <v>30</v>
@@ -828,12 +961,12 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -850,10 +983,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9DD4A9-7F47-415E-AA8D-1892EEF1F04A}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -899,13 +1032,13 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
         <v>32</v>
@@ -913,7 +1046,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E4" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -921,23 +1054,23 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -945,23 +1078,66 @@
         <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D21" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -972,4 +1148,95 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D9F28F-7C55-4742-8172-BEAD018722B9}">
+  <dimension ref="B2:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="28.1796875" style="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B2" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B3" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B4" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B5" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B6" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B7" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B8" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B9" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B10" s="11"/>
+    </row>
+    <row r="11" spans="2:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B11" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="B12" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="B13" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B14" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B15" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B16" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
publication method signatures created
</commit_message>
<xml_diff>
--- a/User Stories/Driver&PubUserStories.xlsx
+++ b/User Stories/Driver&PubUserStories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbcdef5057a82b24/Documents/GitHub/Newsagent-Project/User Stories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="13_ncr:1_{394DACC3-B259-496C-B6F7-60447024E19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA6AE2C1-4B68-4B4A-A623-7D8ADDC06023}"/>
+  <xr:revisionPtr revIDLastSave="141" documentId="13_ncr:1_{394DACC3-B259-496C-B6F7-60447024E19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{537BF5E2-B706-4045-8F8E-EDAECA2E9AD7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{6F4168C7-28B8-4B96-A04E-7170FD7B4563}"/>
   </bookViews>
@@ -290,7 +290,7 @@
     <t>+updateStock() : void</t>
   </si>
   <si>
-    <t>+updateCustomer (id: int, title: String, issueNo: int, author: String, price: double, quantity: int)</t>
+    <t>+updatePublication (id: int, title: String, issueNo: int, author: String, price: double, quantity: int)</t>
   </si>
 </sst>
 </file>
@@ -400,15 +400,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -422,6 +413,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -774,15 +774,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="14" t="s">
         <v>15</v>
       </c>
     </row>
@@ -796,8 +796,8 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="7"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="14"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -1002,15 +1002,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="14" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1024,8 +1024,8 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -1154,85 +1154,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D9F28F-7C55-4742-8172-BEAD018722B9}">
   <dimension ref="B2:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="28.1796875" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B10" s="11"/>
+      <c r="B10" s="8"/>
     </row>
     <row r="11" spans="2:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="9" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="12" spans="2:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="9" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="13" spans="2:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="10" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="8" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="11" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>